<commit_message>
Minor changes to hex codes
</commit_message>
<xml_diff>
--- a/amo/hexCodes/Employee_Status.xlsx
+++ b/amo/hexCodes/Employee_Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrkh\Desktop\YelloCo\5.Fifth Task\AMSServices\amo\hexCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545AD484-0F28-4681-99A1-8CBF290D550C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1E3FE4-B4FA-4C7D-9EF4-A98792BE1930}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Code</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Suspended</t>
+  </si>
+  <si>
+    <t>Assigned but not busy</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,12 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C7" s="1"/>
     </row>
   </sheetData>

</xml_diff>